<commit_message>
Develop TiTle ~ Main Field
Update CutScene
- Add Skip Button
- Add Skip Input

Update Audio Slider (Save, Load, Toggle)

Add TimeScaleHelper (Stack)

Update InputActions (Stack)

Add CheckUIManager

Update Player Interaction

Add Font DoveMayo

Fix Errors
Highlight Item - Selected > Mouse Highlight > DeSelect -> Error (Not Update)
Dialogue - Fix Character Animation
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9278E7EA-69ED-4918-A382-AD9594FDFF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2595DD-552C-448C-8E4C-8D431124570D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -242,7 +242,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -656,7 +656,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -672,7 +672,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{498E9EB0-1553-403F-B471-AA7FB481F786}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{3ADCBB47-357E-40A4-AAC5-1E568139E75B}">
       <text>
         <r>
           <rPr>
@@ -869,7 +869,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -877,7 +877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{96CAF562-77F6-435F-BD7F-4EE7FFC762AE}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{5BF35F2C-3D01-4815-94B3-BEFE2B1EF29A}">
       <text>
         <r>
           <rPr>
@@ -900,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{E877F47A-1FC9-43CC-921A-86FCDD1D8E03}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{47B3F92C-38B3-4F6F-B8D3-FF53BF66BDB4}">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1013,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{0627A2CF-6227-4830-9906-94C6DC94BB64}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{ACF9F59F-876B-42A0-BF4D-3A0B982A72BB}">
       <text>
         <r>
           <rPr>
@@ -1283,7 +1283,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -1299,7 +1299,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{5B698EC1-A640-4993-8E91-CFBCD8C3C964}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{9DF3D2CD-3DB0-45B1-9A8B-6613B1C720AE}">
       <text>
         <r>
           <rPr>
@@ -1496,7 +1496,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -1504,7 +1504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3BDFBF3F-7D5B-4AFB-BAEF-1010D8081A9D}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{80AA2B2B-65C6-4792-BC4C-E7D4CE2B011C}">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{35A053BE-AC05-4B14-A6C1-1802AFB44D52}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{D1252488-E321-4764-9C3F-788563921961}">
       <text>
         <r>
           <rPr>
@@ -1640,7 +1640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{C9A24704-A57C-4B30-994E-08C1DD03FE03}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{A03264A6-7803-4BC4-A4CE-18BD3B2384A3}">
       <text>
         <r>
           <rPr>
@@ -1910,7 +1910,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -1926,7 +1926,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{8ABBAB43-E2E9-46E3-9B7C-0ABE1D5EBEE7}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{D11D9696-1626-4FA1-989A-2DEDAE2F40B6}">
       <text>
         <r>
           <rPr>
@@ -2123,7 +2123,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -2131,7 +2131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3F0B315B-85E7-43D8-AA89-EE209E425199}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{FA34427C-159A-4CE8-8C1E-201302D6D894}">
       <text>
         <r>
           <rPr>
@@ -2154,7 +2154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{C0FA0F43-2401-46CE-A7C2-21180200D58B}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{240FE18A-38BF-48C0-B531-C5F7B3968F73}">
       <text>
         <r>
           <rPr>
@@ -2267,7 +2267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{D1F54D19-A034-4EFA-8F91-AB038A0AB885}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{7DE9A465-774E-478B-B029-41E5D2FFBD6C}">
       <text>
         <r>
           <rPr>
@@ -2537,7 +2537,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -2553,7 +2553,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{CE590442-47B2-47DB-B747-B586585B938B}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{0A2998FF-3160-4987-894A-9B387EB644D0}">
       <text>
         <r>
           <rPr>
@@ -2750,7 +2750,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -2758,7 +2758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{1647D649-F159-4DE1-9A32-D5E1CF44D359}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C381F002-8D0C-45FC-A69C-1590362A4DEE}">
       <text>
         <r>
           <rPr>
@@ -2781,7 +2781,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9569BD11-38E1-47FB-92F5-97FFB1029E72}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9F34C390-C0D1-4FAC-8898-A0E781E0048C}">
       <text>
         <r>
           <rPr>
@@ -2894,7 +2894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{7949C15A-0451-4294-A616-45474764CCC4}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{6B5210AD-76D1-4D1E-884E-EFEB0BA4197C}">
       <text>
         <r>
           <rPr>
@@ -3164,7 +3164,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -3180,7 +3180,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{67C9E311-B170-4226-B16C-E156F4CA4BD2}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{65047D2A-113E-47D5-88B5-D93760949339}">
       <text>
         <r>
           <rPr>
@@ -3377,7 +3377,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -3385,7 +3385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{ADEBC459-7FF0-4CBC-9C38-B2E530DC21FE}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{EAC96702-E8B5-48C0-A46E-59AEC199021C}">
       <text>
         <r>
           <rPr>
@@ -3408,7 +3408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9D24C82E-4EAD-4613-8F55-7291FA945994}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{5A53DC36-CDA6-4938-80C8-0CB283FF1961}">
       <text>
         <r>
           <rPr>
@@ -3521,7 +3521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{88CAFF40-CA00-4EBB-9FAB-1DD0968863C5}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{9BFEC8A9-8528-4989-9F64-9E707EA5B744}">
       <text>
         <r>
           <rPr>
@@ -3791,7 +3791,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="127">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4523,11 +4523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(컷 씬)&gt; (컷 씬 전환): 주인공은 나루와 손을 잡고 주인공의 목걸이에서는 기묘한 빛이 난다.
-(컷 씬)&gt; (컷 씬 전환): 가정집으로 보이는 공간.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 가정집 배경 속 강아지와 그 앞의 밥그릇이 보인다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4546,10 +4541,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Left, Disappear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4597,6 +4588,29 @@
   </si>
   <si>
     <t>SmallRoomScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right,Appear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이와 같은 경우 첫 대사에서 Left, Appear과 Right Appear이 동시에 작동합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(컷 씬)&gt; (컷 씬 전환): 가정집으로 보이는 공간.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(컷 씬)&gt; (컷 씬 전환): 주인공은 나루와 손을 잡고 주인공의 목걸이에서는 기묘한 빛이 난다.</t>
+  </si>
+  <si>
+    <t>Hold, 1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5064,20 +5078,20 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5097,7 +5111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5117,7 +5131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5135,6 +5149,90 @@
       </c>
       <c r="F4" t="s">
         <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5148,8 +5246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5164,7 +5262,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -5257,6 +5355,9 @@
       </c>
       <c r="D6">
         <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -5434,7 +5535,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="33">
@@ -5591,7 +5692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5605,7 +5706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="115.5">
+    <row r="34" spans="1:4" ht="115.5">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -5619,7 +5720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="33">
+    <row r="35" spans="1:4" ht="33">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -5633,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="49.5">
+    <row r="36" spans="1:4" ht="49.5">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -5647,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -5661,7 +5762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -5675,12 +5776,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:4">
       <c r="C39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="66">
+    <row r="40" spans="1:4" ht="66">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -5692,9 +5793,6 @@
       </c>
       <c r="D40">
         <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5706,10 +5804,1369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CC2C1E-6D25-4DF6-8735-FDEFE9F7599E}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="33">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="33">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="82.5">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="49.5">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="66">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="5"/>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" ht="49.5">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" ht="66">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" s="5"/>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" ht="51.75" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="6">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="33">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="6">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="66">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="115.5">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="66">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="33">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="49.5">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="6">
+        <v>6</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="49.5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="66">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="82.5">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="33">
+      <c r="B33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="49.5">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="33">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="82.5">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="6">
+        <v>6</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="99">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="49.5">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="33">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" ht="82.5">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="33">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" ht="49.5">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" ht="33">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="82.5">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="6"/>
+      <c r="B53" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="6">
+        <v>6</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="99">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="49.5">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" ht="33">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" ht="33">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" ht="99">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" ht="49.5">
+      <c r="A61" s="6"/>
+      <c r="B61" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="6">
+        <v>6</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" ht="33">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" ht="33">
+      <c r="A64" s="6"/>
+      <c r="B64" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="6">
+        <v>6</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D80C0E-6C2C-4983-9442-683187F41940}">
+  <dimension ref="A1:P63"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="82.5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="82.5">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="49.5">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
+  <dimension ref="A1:P61"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5788,1341 +7245,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="33">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="33">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="82.5">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="49.5">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="66">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="B11" s="5"/>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" ht="49.5">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" ht="66">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="5"/>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" ht="82.5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="6">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="66">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="115.5">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="66">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="33">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="49.5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="6">
-        <v>6</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="49.5">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="66">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="82.5">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="33">
-      <c r="B32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="49.5">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="33">
-      <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="82.5">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="6">
-        <v>6</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="99">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="49.5">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="33">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="82.5">
-      <c r="A44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" ht="33">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="49.5">
-      <c r="A48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" ht="33">
-      <c r="A49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" ht="82.5">
-      <c r="A50" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="6"/>
-      <c r="B52" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="6">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" ht="99">
-      <c r="A53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" ht="49.5">
-      <c r="A54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" ht="33">
-      <c r="A55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="B56" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" ht="33">
-      <c r="A58" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" ht="99">
-      <c r="A59" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" ht="49.5">
-      <c r="A60" s="6"/>
-      <c r="B60" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="6">
-        <v>6</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" ht="33">
-      <c r="A62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" ht="33">
-      <c r="A63" s="6"/>
-      <c r="B63" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="6">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D80C0E-6C2C-4983-9442-683187F41940}">
-  <dimension ref="A1:P63"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>114</v>
-      </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="82.5">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="82.5">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="49.5">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="2"/>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
-  <dimension ref="A1:P61"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>115</v>
-      </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>27</v>
@@ -7170,7 +7292,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="6">
         <v>4</v>

</xml_diff>

<commit_message>
Develop TiTle ~ Main Field (#41)
Update CutScene
- Add Skip Button
- Add Skip Input

Update Audio Slider (Save, Load, Toggle)

Add TimeScaleHelper (Stack)

Update InputActions (Stack)

Add CheckUIManager

Update Player Interaction

Add Font DoveMayo

Fix Errors
Highlight Item - Selected > Mouse Highlight > DeSelect -> Error (Not Update)
Dialogue - Fix Character Animation
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9278E7EA-69ED-4918-A382-AD9594FDFF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2595DD-552C-448C-8E4C-8D431124570D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -242,7 +242,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -656,7 +656,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -672,7 +672,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{498E9EB0-1553-403F-B471-AA7FB481F786}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{3ADCBB47-357E-40A4-AAC5-1E568139E75B}">
       <text>
         <r>
           <rPr>
@@ -869,7 +869,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -877,7 +877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{96CAF562-77F6-435F-BD7F-4EE7FFC762AE}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{5BF35F2C-3D01-4815-94B3-BEFE2B1EF29A}">
       <text>
         <r>
           <rPr>
@@ -900,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{E877F47A-1FC9-43CC-921A-86FCDD1D8E03}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{47B3F92C-38B3-4F6F-B8D3-FF53BF66BDB4}">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1013,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{0627A2CF-6227-4830-9906-94C6DC94BB64}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{ACF9F59F-876B-42A0-BF4D-3A0B982A72BB}">
       <text>
         <r>
           <rPr>
@@ -1283,7 +1283,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -1299,7 +1299,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{5B698EC1-A640-4993-8E91-CFBCD8C3C964}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{9DF3D2CD-3DB0-45B1-9A8B-6613B1C720AE}">
       <text>
         <r>
           <rPr>
@@ -1496,7 +1496,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -1504,7 +1504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3BDFBF3F-7D5B-4AFB-BAEF-1010D8081A9D}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{80AA2B2B-65C6-4792-BC4C-E7D4CE2B011C}">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{35A053BE-AC05-4B14-A6C1-1802AFB44D52}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{D1252488-E321-4764-9C3F-788563921961}">
       <text>
         <r>
           <rPr>
@@ -1640,7 +1640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{C9A24704-A57C-4B30-994E-08C1DD03FE03}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{A03264A6-7803-4BC4-A4CE-18BD3B2384A3}">
       <text>
         <r>
           <rPr>
@@ -1910,7 +1910,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -1926,7 +1926,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{8ABBAB43-E2E9-46E3-9B7C-0ABE1D5EBEE7}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{D11D9696-1626-4FA1-989A-2DEDAE2F40B6}">
       <text>
         <r>
           <rPr>
@@ -2123,7 +2123,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -2131,7 +2131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3F0B315B-85E7-43D8-AA89-EE209E425199}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{FA34427C-159A-4CE8-8C1E-201302D6D894}">
       <text>
         <r>
           <rPr>
@@ -2154,7 +2154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{C0FA0F43-2401-46CE-A7C2-21180200D58B}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{240FE18A-38BF-48C0-B531-C5F7B3968F73}">
       <text>
         <r>
           <rPr>
@@ -2267,7 +2267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{D1F54D19-A034-4EFA-8F91-AB038A0AB885}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{7DE9A465-774E-478B-B029-41E5D2FFBD6C}">
       <text>
         <r>
           <rPr>
@@ -2537,7 +2537,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -2553,7 +2553,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{CE590442-47B2-47DB-B747-B586585B938B}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{0A2998FF-3160-4987-894A-9B387EB644D0}">
       <text>
         <r>
           <rPr>
@@ -2750,7 +2750,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -2758,7 +2758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{1647D649-F159-4DE1-9A32-D5E1CF44D359}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C381F002-8D0C-45FC-A69C-1590362A4DEE}">
       <text>
         <r>
           <rPr>
@@ -2781,7 +2781,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9569BD11-38E1-47FB-92F5-97FFB1029E72}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9F34C390-C0D1-4FAC-8898-A0E781E0048C}">
       <text>
         <r>
           <rPr>
@@ -2894,7 +2894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{7949C15A-0451-4294-A616-45474764CCC4}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{6B5210AD-76D1-4D1E-884E-EFEB0BA4197C}">
       <text>
         <r>
           <rPr>
@@ -3164,7 +3164,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -3180,7 +3180,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{67C9E311-B170-4226-B16C-E156F4CA4BD2}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{65047D2A-113E-47D5-88B5-D93760949339}">
       <text>
         <r>
           <rPr>
@@ -3377,7 +3377,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute
+11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -3385,7 +3385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{ADEBC459-7FF0-4CBC-9C38-B2E530DC21FE}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{EAC96702-E8B5-48C0-A46E-59AEC199021C}">
       <text>
         <r>
           <rPr>
@@ -3408,7 +3408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9D24C82E-4EAD-4613-8F55-7291FA945994}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{5A53DC36-CDA6-4938-80C8-0CB283FF1961}">
       <text>
         <r>
           <rPr>
@@ -3521,7 +3521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{88CAFF40-CA00-4EBB-9FAB-1DD0968863C5}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{9BFEC8A9-8528-4989-9F64-9E707EA5B744}">
       <text>
         <r>
           <rPr>
@@ -3791,7 +3791,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="127">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4523,11 +4523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(컷 씬)&gt; (컷 씬 전환): 주인공은 나루와 손을 잡고 주인공의 목걸이에서는 기묘한 빛이 난다.
-(컷 씬)&gt; (컷 씬 전환): 가정집으로 보이는 공간.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 가정집 배경 속 강아지와 그 앞의 밥그릇이 보인다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4546,10 +4541,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Left, Disappear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4597,6 +4588,29 @@
   </si>
   <si>
     <t>SmallRoomScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right,Appear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이와 같은 경우 첫 대사에서 Left, Appear과 Right Appear이 동시에 작동합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(컷 씬)&gt; (컷 씬 전환): 가정집으로 보이는 공간.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(컷 씬)&gt; (컷 씬 전환): 주인공은 나루와 손을 잡고 주인공의 목걸이에서는 기묘한 빛이 난다.</t>
+  </si>
+  <si>
+    <t>Hold, 1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5064,20 +5078,20 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5097,7 +5111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5117,7 +5131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5135,6 +5149,90 @@
       </c>
       <c r="F4" t="s">
         <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5148,8 +5246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5164,7 +5262,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -5257,6 +5355,9 @@
       </c>
       <c r="D6">
         <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -5434,7 +5535,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="33">
@@ -5591,7 +5692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5605,7 +5706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="115.5">
+    <row r="34" spans="1:4" ht="115.5">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -5619,7 +5720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="33">
+    <row r="35" spans="1:4" ht="33">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -5633,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="49.5">
+    <row r="36" spans="1:4" ht="49.5">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -5647,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -5661,7 +5762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -5675,12 +5776,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:4">
       <c r="C39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="66">
+    <row r="40" spans="1:4" ht="66">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -5692,9 +5793,6 @@
       </c>
       <c r="D40">
         <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5706,10 +5804,1369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CC2C1E-6D25-4DF6-8735-FDEFE9F7599E}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="33">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="33">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="82.5">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="49.5">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="66">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="5"/>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" ht="49.5">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" ht="66">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" s="5"/>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" ht="51.75" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="6">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="33">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="6">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="66">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="115.5">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="66">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="33">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="49.5">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="6">
+        <v>6</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="49.5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="66">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="82.5">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="33">
+      <c r="B33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="49.5">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="33">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="82.5">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="6">
+        <v>6</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="99">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="49.5">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="33">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" ht="82.5">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="33">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" ht="49.5">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" ht="33">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="82.5">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="6"/>
+      <c r="B53" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="6">
+        <v>6</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="99">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="49.5">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" ht="33">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" ht="33">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" ht="99">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" ht="49.5">
+      <c r="A61" s="6"/>
+      <c r="B61" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="6">
+        <v>6</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" ht="33">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" ht="33">
+      <c r="A64" s="6"/>
+      <c r="B64" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="6">
+        <v>6</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D80C0E-6C2C-4983-9442-683187F41940}">
+  <dimension ref="A1:P63"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="82.5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="82.5">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="49.5">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
+  <dimension ref="A1:P61"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5788,1341 +7245,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="33">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="33">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="82.5">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="49.5">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="66">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="B11" s="5"/>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" ht="49.5">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" ht="66">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="5"/>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" ht="82.5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="6">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="66">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="115.5">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="66">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="33">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="49.5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="6">
-        <v>6</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="49.5">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="66">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="82.5">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="33">
-      <c r="B32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="49.5">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="33">
-      <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="82.5">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="6">
-        <v>6</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="99">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="49.5">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="33">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="82.5">
-      <c r="A44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" ht="33">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="49.5">
-      <c r="A48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" ht="33">
-      <c r="A49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" ht="82.5">
-      <c r="A50" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="6"/>
-      <c r="B52" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="6">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" ht="99">
-      <c r="A53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" ht="49.5">
-      <c r="A54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" ht="33">
-      <c r="A55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="B56" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" ht="33">
-      <c r="A58" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" ht="99">
-      <c r="A59" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" ht="49.5">
-      <c r="A60" s="6"/>
-      <c r="B60" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="6">
-        <v>6</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" ht="33">
-      <c r="A62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" ht="33">
-      <c r="A63" s="6"/>
-      <c r="B63" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="6">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D80C0E-6C2C-4983-9442-683187F41940}">
-  <dimension ref="A1:P63"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>114</v>
-      </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="82.5">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="82.5">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="49.5">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="2"/>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
-  <dimension ref="A1:P61"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>115</v>
-      </c>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>27</v>
@@ -7170,7 +7292,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="6">
         <v>4</v>

</xml_diff>

<commit_message>
Add SmallRoomScene Prototype (#56)
* Add SmallRoomScene Prototype

* Add Open Scene
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2595DD-552C-448C-8E4C-8D431124570D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4955FC4C-122D-404F-ADAB-DD26C14C228C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <author>서 의수</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{3ACC3B38-DE92-45C1-8270-F6458F77132A}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{D1BEF015-2224-4301-82B9-B650867B9DFF}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
 5: Save
 9: Random
 10: Random End
-11: Immediately Execute (대사 없이 바로 캐릭터 State를 변경하는 용도로 사용합니다. ex) Left, Appear와 Right, Appear를 동시에 사용하고 싶은 경우)
+11: Immediately Execute
 // Inspector창에서 직접 조정
 6: CutScene
 7: WaitInteract
@@ -250,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{55F3406C-DD2D-4558-AA61-7ED1D57CC430}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{4E42F7AA-E7BC-4A7B-A16F-366053596261}">
       <text>
         <r>
           <rPr>
@@ -273,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{EB430104-7C44-425D-816D-8017353F3388}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{FC26E258-34AA-4B78-B60C-093F2C4B278A}">
       <text>
         <r>
           <rPr>
@@ -386,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{8E68F913-8DAB-482A-B615-15A1F117EB23}">
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{00B050FC-4356-42BF-8968-193B15AD8ABC}">
       <text>
         <r>
           <rPr>
@@ -656,7 +656,7 @@
 v0, v1, v2, v3 (순서 무관)
 v0 - Hold, None (Default - None)   (대소문자 무관)
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
-v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
+v2 - true, false 다음 Index로 Auto 여부 (Default - true)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
         </r>
       </text>
@@ -5080,8 +5080,8 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:F4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5246,7 +5246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Excel (Character Naming)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5907C6-A5B5-46FB-8E4A-6FED949333A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BE8F7-563F-4F3C-9723-CB9B00F469E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="160">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3872,9 +3872,6 @@
   <si>
     <t>enum:Expression:Keep</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주인공</t>
   </si>
   <si>
     <t>주인공</t>
@@ -4026,48 +4023,6 @@
   <si>
     <t>모두들 그렇게 이야기하더라. 기억이 온전치 않은데도.
 참 이상한 일이지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>그다지 특별한 일은 아니지. 오히려 종종 있던 일 이라고 할까?
-물론, 완전히 기억이 없는 경우는 흔하지 않지만.
-우리는 그들을 &lt;b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘길을 잃은 사람들’</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>이라고 불러.</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4716,6 +4671,51 @@
   </si>
   <si>
     <t>Hold, 0.1, name=Main/Prologue/#2-2 Remove Naru Doll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그다지 특별한 일은 아니지. 오히려 종종 있던 일 이라고 할까?
+물론, 완전히 기억이 없는 경우는 흔하지 않지만.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>우리는 그들을 &lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>‘길을 잃은 사람들’</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이라고 불러.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4926,15 +4926,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -4942,6 +4933,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5271,7 +5271,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5334,15 +5334,15 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5359,15 +5359,15 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5378,10 +5378,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5392,10 +5392,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5406,10 +5406,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -5427,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5444,7 +5444,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -5509,561 +5509,575 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="17">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="17">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17">
+        <v>2</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17">
+        <v>3</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17">
+        <v>2</v>
+      </c>
+      <c r="D9" s="17">
+        <v>2</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17">
+        <v>3</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" ht="49.5">
+      <c r="A11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="17">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" ht="66">
+      <c r="A12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" ht="33">
+      <c r="A13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="17">
+        <v>1</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="17">
+        <v>2</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17">
+        <v>3</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" ht="49.5">
+      <c r="A16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="17">
+        <v>1</v>
+      </c>
+      <c r="D16" s="17">
+        <v>3</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="33">
+      <c r="A17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="49.5">
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="17">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="33">
+      <c r="A20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="17">
+        <v>1</v>
+      </c>
+      <c r="D20" s="17">
+        <v>3</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" ht="49.5">
+      <c r="A21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="C21" s="17">
+        <v>1</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" ht="33">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="17">
+        <v>6</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="33">
+      <c r="A23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="17">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" ht="33">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="17">
+        <v>6</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="17">
         <v>2</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="17">
+        <v>2</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="14" t="s">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="49.5">
+      <c r="A28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="17">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="17">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17">
+        <v>2</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="66">
+      <c r="A30" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="17">
+        <v>1</v>
+      </c>
+      <c r="D30" s="17">
+        <v>3</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C31" s="17">
+        <v>1</v>
+      </c>
+      <c r="D31" s="17">
         <v>2</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" ht="33">
+      <c r="A32" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="17">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17">
         <v>3</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" ht="66">
+      <c r="A33" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="17">
+        <v>1</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" spans="1:6" ht="82.5">
+      <c r="A34" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="17">
+        <v>1</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="17">
+        <v>1</v>
+      </c>
+      <c r="D35" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="14">
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" ht="33">
+      <c r="A36" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="17">
+        <v>1</v>
+      </c>
+      <c r="D36" s="17">
+        <v>3</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" ht="49.5">
+      <c r="A37" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="17">
+        <v>1</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+      <c r="D38" s="17">
         <v>2</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14">
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6" ht="49.5">
+      <c r="A39" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="17">
+        <v>1</v>
+      </c>
+      <c r="D39" s="17">
         <v>3</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:16" ht="49.5">
-      <c r="A11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="17">
+        <v>2</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="17">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17">
         <v>3</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:16" ht="99">
-      <c r="A12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="14">
-        <v>1</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="14">
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" ht="49.5">
+      <c r="A43" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="17">
+        <v>1</v>
+      </c>
+      <c r="D43" s="17">
         <v>2</v>
       </c>
-      <c r="D13" s="14">
-        <v>2</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:16" ht="49.5">
-      <c r="A15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14">
-        <v>3</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" ht="33">
-      <c r="A16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="49.5">
-      <c r="A17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
-      <c r="D18" s="14">
-        <v>2</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="33">
-      <c r="A19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="14">
-        <v>3</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="49.5">
-      <c r="A20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" ht="33">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="14">
-        <v>6</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="33">
-      <c r="A22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" ht="33">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="14">
-        <v>6</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="14">
-        <v>2</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="14">
-        <v>2</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14">
-        <v>3</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="49.5">
-      <c r="A27" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="14">
-        <v>1</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="14">
-        <v>1</v>
-      </c>
-      <c r="D28" s="14">
-        <v>2</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="66">
-      <c r="A29" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="14">
-        <v>1</v>
-      </c>
-      <c r="D29" s="14">
-        <v>3</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="14">
-        <v>1</v>
-      </c>
-      <c r="D30" s="14">
-        <v>2</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" ht="33">
-      <c r="A31" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="14">
-        <v>1</v>
-      </c>
-      <c r="D31" s="14">
-        <v>3</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:6" ht="66">
-      <c r="A32" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="14">
-        <v>1</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" ht="82.5">
-      <c r="A33" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="14">
-        <v>1</v>
-      </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="14">
-        <v>1</v>
-      </c>
-      <c r="D34" s="14">
-        <v>2</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" ht="33">
-      <c r="A35" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="14">
-        <v>1</v>
-      </c>
-      <c r="D35" s="14">
-        <v>3</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:6" ht="49.5">
-      <c r="A36" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="14">
-        <v>1</v>
-      </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="14">
-        <v>1</v>
-      </c>
-      <c r="D37" s="14">
-        <v>2</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:6" ht="49.5">
-      <c r="A38" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="14">
-        <v>1</v>
-      </c>
-      <c r="D38" s="14">
-        <v>3</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="14"/>
-      <c r="B39" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="14">
-        <v>2</v>
-      </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="14">
-        <v>2</v>
-      </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14">
-        <v>3</v>
-      </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="1:6" ht="49.5">
-      <c r="A42" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="14">
-        <v>1</v>
-      </c>
-      <c r="D42" s="14">
-        <v>2</v>
-      </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14">
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17">
         <v>11</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14" t="s">
-        <v>78</v>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -6077,7 +6091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CC2C1E-6D25-4DF6-8735-FDEFE9F7599E}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6093,7 +6107,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -6160,7 +6174,7 @@
     <row r="5" spans="1:16" ht="33">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7">
         <v>6</v>
@@ -6168,7 +6182,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -6187,10 +6201,10 @@
     </row>
     <row r="7" spans="1:16" ht="33">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -6204,10 +6218,10 @@
     </row>
     <row r="8" spans="1:16" ht="82.5">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
@@ -6219,10 +6233,10 @@
     </row>
     <row r="9" spans="1:16" ht="49.5">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -6234,10 +6248,10 @@
     </row>
     <row r="10" spans="1:16" ht="66">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -6250,7 +6264,7 @@
     <row r="11" spans="1:16">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -6273,10 +6287,10 @@
     </row>
     <row r="13" spans="1:16" ht="49.5">
       <c r="A13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -6288,10 +6302,10 @@
     </row>
     <row r="14" spans="1:16" ht="66">
       <c r="A14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -6304,7 +6318,7 @@
     <row r="15" spans="1:16">
       <c r="A15" s="9"/>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
@@ -6328,7 +6342,7 @@
     <row r="17" spans="1:8" ht="51.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="7">
         <v>6</v>
@@ -6336,14 +6350,14 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="33">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="7">
         <v>6</v>
@@ -6351,16 +6365,16 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -6375,7 +6389,7 @@
     <row r="20" spans="1:8">
       <c r="A20" s="9"/>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
@@ -6388,7 +6402,7 @@
     <row r="21" spans="1:8">
       <c r="A21" s="9"/>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -6401,7 +6415,7 @@
     <row r="22" spans="1:8">
       <c r="A22" s="9"/>
       <c r="B22" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="9">
         <v>3</v>
@@ -6413,10 +6427,10 @@
     </row>
     <row r="23" spans="1:8" ht="66">
       <c r="A23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -6430,10 +6444,10 @@
     </row>
     <row r="24" spans="1:8" ht="66">
       <c r="A24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -6445,10 +6459,10 @@
     </row>
     <row r="25" spans="1:8" ht="49.5">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -6460,10 +6474,10 @@
     </row>
     <row r="26" spans="1:8" ht="66">
       <c r="A26" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -6475,10 +6489,10 @@
     </row>
     <row r="27" spans="1:8" ht="33">
       <c r="A27" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -6491,7 +6505,7 @@
     <row r="28" spans="1:8" ht="49.5">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7">
         <v>6</v>
@@ -6499,16 +6513,16 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -6520,10 +6534,10 @@
     </row>
     <row r="30" spans="1:8" ht="49.5">
       <c r="A30" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -6535,10 +6549,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -6550,10 +6564,10 @@
     </row>
     <row r="32" spans="1:8" ht="66">
       <c r="A32" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -6565,10 +6579,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
@@ -6580,10 +6594,10 @@
     </row>
     <row r="34" spans="1:8" ht="82.5">
       <c r="A34" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="10">
         <v>1</v>
@@ -6595,10 +6609,10 @@
     </row>
     <row r="35" spans="1:8" ht="33">
       <c r="A35" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -6610,10 +6624,10 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="10">
         <v>1</v>
@@ -6625,10 +6639,10 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="10">
         <v>1</v>
@@ -6640,10 +6654,10 @@
     </row>
     <row r="38" spans="1:8" ht="49.5">
       <c r="A38" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C38" s="10">
         <v>1</v>
@@ -6655,10 +6669,10 @@
     </row>
     <row r="39" spans="1:8" ht="33">
       <c r="A39" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" s="10">
         <v>1</v>
@@ -6670,10 +6684,10 @@
     </row>
     <row r="40" spans="1:8" ht="82.5">
       <c r="A40" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
@@ -6685,10 +6699,10 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="C41" s="10">
         <v>1</v>
@@ -6701,7 +6715,7 @@
     <row r="42" spans="1:8">
       <c r="A42" s="11"/>
       <c r="B42" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="10">
         <v>6</v>
@@ -6709,16 +6723,16 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" ht="49.5">
       <c r="A43" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" s="10">
         <v>1</v>
@@ -6728,16 +6742,16 @@
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8" ht="49.5">
       <c r="A44" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C44" s="10">
         <v>1</v>
@@ -6749,10 +6763,10 @@
     </row>
     <row r="45" spans="1:8" ht="33">
       <c r="A45" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="10">
         <v>1</v>
@@ -6765,7 +6779,7 @@
     <row r="46" spans="1:8">
       <c r="A46" s="12"/>
       <c r="B46" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="12">
         <v>2</v>
@@ -6777,10 +6791,10 @@
     </row>
     <row r="47" spans="1:8" ht="82.5">
       <c r="A47" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" s="12">
         <v>1</v>
@@ -6792,10 +6806,10 @@
     </row>
     <row r="48" spans="1:8" ht="33">
       <c r="A48" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="12">
         <v>1</v>
@@ -6807,10 +6821,10 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -6822,10 +6836,10 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
@@ -6839,10 +6853,10 @@
     </row>
     <row r="51" spans="1:8" ht="49.5">
       <c r="A51" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
@@ -6856,10 +6870,10 @@
     </row>
     <row r="52" spans="1:8" ht="33">
       <c r="A52" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
@@ -6873,10 +6887,10 @@
     </row>
     <row r="53" spans="1:8" ht="82.5">
       <c r="A53" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
@@ -6890,10 +6904,10 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
@@ -6908,7 +6922,7 @@
     <row r="55" spans="1:8">
       <c r="A55" s="12"/>
       <c r="B55" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" s="12">
         <v>6</v>
@@ -6916,16 +6930,16 @@
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" ht="49.5">
       <c r="A56" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C56" s="12">
         <v>1</v>
@@ -6935,16 +6949,16 @@
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" ht="49.5">
       <c r="A57" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -6956,10 +6970,10 @@
     </row>
     <row r="58" spans="1:8" ht="49.5">
       <c r="A58" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="12">
         <v>1</v>
@@ -6971,10 +6985,10 @@
     </row>
     <row r="59" spans="1:8" ht="33">
       <c r="A59" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -6987,7 +7001,7 @@
     <row r="60" spans="1:8">
       <c r="A60" s="9"/>
       <c r="B60" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="9">
         <v>3</v>
@@ -7067,7 +7081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17942C2D-E350-4175-91DA-E8D32862B86D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -7082,7 +7096,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7146,277 +7160,277 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="17">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="A5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
-        <v>79</v>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33">
-      <c r="A6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="33">
+      <c r="A7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="33">
+      <c r="A8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="33">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="17">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17">
+      <c r="C9" s="14">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="33">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="14">
+        <v>6</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="49.5">
+      <c r="A13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
         <v>3</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" ht="33">
-      <c r="A7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="17">
-        <v>1</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" ht="33">
-      <c r="A8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="17">
-        <v>1</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="33">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="17">
-        <v>6</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="17">
-        <v>1</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14">
         <v>2</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" ht="33">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="17">
-        <v>6</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="49.5">
-      <c r="A13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="19" t="s">
+      <c r="B17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="49.5">
+      <c r="A19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="33">
+      <c r="A20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="17">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17">
-        <v>3</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="17">
-        <v>1</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
         <v>2</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="17">
-        <v>1</v>
-      </c>
-      <c r="D15" s="17">
-        <v>3</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="17">
-        <v>1</v>
-      </c>
-      <c r="D16" s="17">
-        <v>2</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="17">
-        <v>3</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="17">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" ht="49.5">
-      <c r="A19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="17">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17">
-        <v>3</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" ht="33">
-      <c r="A20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="17">
-        <v>1</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="17">
-        <v>1</v>
-      </c>
-      <c r="D21" s="17">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14">
         <v>11</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17" t="s">
-        <v>78</v>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -7430,15 +7444,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7503,10 +7517,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7518,15 +7532,15 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7535,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7584,10 +7598,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -7598,10 +7612,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7615,7 +7629,7 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -7627,10 +7641,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -7644,7 +7658,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -7710,10 +7724,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7722,12 +7736,12 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -7735,10 +7749,10 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7747,30 +7761,22 @@
     <row r="8" spans="1:16">
       <c r="B8" s="2"/>
       <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="2"/>
+      <c r="C9">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>148</v>
+      <c r="F9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -7778,13 +7784,13 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
@@ -7792,13 +7798,13 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
@@ -7806,13 +7812,13 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
@@ -7820,13 +7826,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C14" s="2">
         <v>6</v>
@@ -7834,13 +7840,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2">
         <v>6</v>
@@ -7848,13 +7854,13 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -7862,13 +7868,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2">
         <v>6</v>
@@ -7876,110 +7882,117 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
+      <c r="A18" s="2"/>
+      <c r="B18" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
       <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
         <v>11</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="C23" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23">
+    <row r="24" spans="1:6">
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
     <row r="25" spans="1:6">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" s="2"/>
       <c r="C26">
-        <v>11</v>
-      </c>
-      <c r="F26" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="2"/>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" s="2"/>
@@ -8056,8 +8069,8 @@
     <row r="52" spans="2:2">
       <c r="B52" s="2"/>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="2"/>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="2"/>
@@ -8065,14 +8078,17 @@
     <row r="57" spans="2:2">
       <c r="B57" s="2"/>
     </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="2"/>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2"/>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update Excel (Character Naming) (#69)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5907C6-A5B5-46FB-8E4A-6FED949333A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BE8F7-563F-4F3C-9723-CB9B00F469E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="160">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3872,9 +3872,6 @@
   <si>
     <t>enum:Expression:Keep</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주인공</t>
   </si>
   <si>
     <t>주인공</t>
@@ -4026,48 +4023,6 @@
   <si>
     <t>모두들 그렇게 이야기하더라. 기억이 온전치 않은데도.
 참 이상한 일이지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>그다지 특별한 일은 아니지. 오히려 종종 있던 일 이라고 할까?
-물론, 완전히 기억이 없는 경우는 흔하지 않지만.
-우리는 그들을 &lt;b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘길을 잃은 사람들’</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>이라고 불러.</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4716,6 +4671,51 @@
   </si>
   <si>
     <t>Hold, 0.1, name=Main/Prologue/#2-2 Remove Naru Doll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그다지 특별한 일은 아니지. 오히려 종종 있던 일 이라고 할까?
+물론, 완전히 기억이 없는 경우는 흔하지 않지만.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>우리는 그들을 &lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>‘길을 잃은 사람들’</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이라고 불러.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4926,15 +4926,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -4942,6 +4933,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5271,7 +5271,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5334,15 +5334,15 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5359,15 +5359,15 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5378,10 +5378,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5392,10 +5392,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5406,10 +5406,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -5427,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5444,7 +5444,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -5509,561 +5509,575 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="17">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="17">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17">
+        <v>2</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17">
+        <v>3</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17">
+        <v>2</v>
+      </c>
+      <c r="D9" s="17">
+        <v>2</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17">
+        <v>3</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" ht="49.5">
+      <c r="A11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="17">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" ht="66">
+      <c r="A12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" ht="33">
+      <c r="A13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="17">
+        <v>1</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="17">
+        <v>2</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17">
+        <v>3</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" ht="49.5">
+      <c r="A16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="17">
+        <v>1</v>
+      </c>
+      <c r="D16" s="17">
+        <v>3</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="33">
+      <c r="A17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="49.5">
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="17">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="33">
+      <c r="A20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="17">
+        <v>1</v>
+      </c>
+      <c r="D20" s="17">
+        <v>3</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" ht="49.5">
+      <c r="A21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="C21" s="17">
+        <v>1</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" ht="33">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="17">
+        <v>6</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="33">
+      <c r="A23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="17">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" ht="33">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="17">
+        <v>6</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="17">
         <v>2</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="17">
+        <v>2</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="14" t="s">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="49.5">
+      <c r="A28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="17">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="17">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17">
+        <v>2</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="66">
+      <c r="A30" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="17">
+        <v>1</v>
+      </c>
+      <c r="D30" s="17">
+        <v>3</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="14">
-        <v>1</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C31" s="17">
+        <v>1</v>
+      </c>
+      <c r="D31" s="17">
         <v>2</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
-      <c r="D8" s="14">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" ht="33">
+      <c r="A32" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="17">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17">
         <v>3</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" ht="66">
+      <c r="A33" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="17">
+        <v>1</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" spans="1:6" ht="82.5">
+      <c r="A34" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="17">
+        <v>1</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="17">
+        <v>1</v>
+      </c>
+      <c r="D35" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="14">
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" ht="33">
+      <c r="A36" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="17">
+        <v>1</v>
+      </c>
+      <c r="D36" s="17">
+        <v>3</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" ht="49.5">
+      <c r="A37" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="17">
+        <v>1</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+      <c r="D38" s="17">
         <v>2</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14">
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6" ht="49.5">
+      <c r="A39" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="17">
+        <v>1</v>
+      </c>
+      <c r="D39" s="17">
         <v>3</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:16" ht="49.5">
-      <c r="A11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="17">
+        <v>2</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="17">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17">
         <v>3</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:16" ht="99">
-      <c r="A12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="14">
-        <v>1</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="14">
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" ht="49.5">
+      <c r="A43" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="17">
+        <v>1</v>
+      </c>
+      <c r="D43" s="17">
         <v>2</v>
       </c>
-      <c r="D13" s="14">
-        <v>2</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:16" ht="49.5">
-      <c r="A15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14">
-        <v>3</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" ht="33">
-      <c r="A16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="49.5">
-      <c r="A17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
-      <c r="D18" s="14">
-        <v>2</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="33">
-      <c r="A19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="14">
-        <v>3</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="49.5">
-      <c r="A20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" ht="33">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="14">
-        <v>6</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="33">
-      <c r="A22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" ht="33">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="14">
-        <v>6</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="14">
-        <v>2</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="14">
-        <v>2</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14">
-        <v>3</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="49.5">
-      <c r="A27" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="14">
-        <v>1</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="14">
-        <v>1</v>
-      </c>
-      <c r="D28" s="14">
-        <v>2</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="66">
-      <c r="A29" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="14">
-        <v>1</v>
-      </c>
-      <c r="D29" s="14">
-        <v>3</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="14">
-        <v>1</v>
-      </c>
-      <c r="D30" s="14">
-        <v>2</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" ht="33">
-      <c r="A31" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="14">
-        <v>1</v>
-      </c>
-      <c r="D31" s="14">
-        <v>3</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:6" ht="66">
-      <c r="A32" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="14">
-        <v>1</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" ht="82.5">
-      <c r="A33" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="14">
-        <v>1</v>
-      </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="14">
-        <v>1</v>
-      </c>
-      <c r="D34" s="14">
-        <v>2</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" ht="33">
-      <c r="A35" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="14">
-        <v>1</v>
-      </c>
-      <c r="D35" s="14">
-        <v>3</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:6" ht="49.5">
-      <c r="A36" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="14">
-        <v>1</v>
-      </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="14">
-        <v>1</v>
-      </c>
-      <c r="D37" s="14">
-        <v>2</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:6" ht="49.5">
-      <c r="A38" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="14">
-        <v>1</v>
-      </c>
-      <c r="D38" s="14">
-        <v>3</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="14"/>
-      <c r="B39" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="14">
-        <v>2</v>
-      </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="14">
-        <v>2</v>
-      </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14">
-        <v>3</v>
-      </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="1:6" ht="49.5">
-      <c r="A42" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="14">
-        <v>1</v>
-      </c>
-      <c r="D42" s="14">
-        <v>2</v>
-      </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14">
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17">
         <v>11</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14" t="s">
-        <v>78</v>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -6077,7 +6091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CC2C1E-6D25-4DF6-8735-FDEFE9F7599E}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6093,7 +6107,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -6160,7 +6174,7 @@
     <row r="5" spans="1:16" ht="33">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7">
         <v>6</v>
@@ -6168,7 +6182,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -6187,10 +6201,10 @@
     </row>
     <row r="7" spans="1:16" ht="33">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -6204,10 +6218,10 @@
     </row>
     <row r="8" spans="1:16" ht="82.5">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
@@ -6219,10 +6233,10 @@
     </row>
     <row r="9" spans="1:16" ht="49.5">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -6234,10 +6248,10 @@
     </row>
     <row r="10" spans="1:16" ht="66">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -6250,7 +6264,7 @@
     <row r="11" spans="1:16">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -6273,10 +6287,10 @@
     </row>
     <row r="13" spans="1:16" ht="49.5">
       <c r="A13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -6288,10 +6302,10 @@
     </row>
     <row r="14" spans="1:16" ht="66">
       <c r="A14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -6304,7 +6318,7 @@
     <row r="15" spans="1:16">
       <c r="A15" s="9"/>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
@@ -6328,7 +6342,7 @@
     <row r="17" spans="1:8" ht="51.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="7">
         <v>6</v>
@@ -6336,14 +6350,14 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="33">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="7">
         <v>6</v>
@@ -6351,16 +6365,16 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -6375,7 +6389,7 @@
     <row r="20" spans="1:8">
       <c r="A20" s="9"/>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
@@ -6388,7 +6402,7 @@
     <row r="21" spans="1:8">
       <c r="A21" s="9"/>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -6401,7 +6415,7 @@
     <row r="22" spans="1:8">
       <c r="A22" s="9"/>
       <c r="B22" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="9">
         <v>3</v>
@@ -6413,10 +6427,10 @@
     </row>
     <row r="23" spans="1:8" ht="66">
       <c r="A23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -6430,10 +6444,10 @@
     </row>
     <row r="24" spans="1:8" ht="66">
       <c r="A24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -6445,10 +6459,10 @@
     </row>
     <row r="25" spans="1:8" ht="49.5">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -6460,10 +6474,10 @@
     </row>
     <row r="26" spans="1:8" ht="66">
       <c r="A26" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -6475,10 +6489,10 @@
     </row>
     <row r="27" spans="1:8" ht="33">
       <c r="A27" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -6491,7 +6505,7 @@
     <row r="28" spans="1:8" ht="49.5">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7">
         <v>6</v>
@@ -6499,16 +6513,16 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -6520,10 +6534,10 @@
     </row>
     <row r="30" spans="1:8" ht="49.5">
       <c r="A30" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -6535,10 +6549,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -6550,10 +6564,10 @@
     </row>
     <row r="32" spans="1:8" ht="66">
       <c r="A32" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -6565,10 +6579,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
@@ -6580,10 +6594,10 @@
     </row>
     <row r="34" spans="1:8" ht="82.5">
       <c r="A34" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="10">
         <v>1</v>
@@ -6595,10 +6609,10 @@
     </row>
     <row r="35" spans="1:8" ht="33">
       <c r="A35" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -6610,10 +6624,10 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="10">
         <v>1</v>
@@ -6625,10 +6639,10 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="10">
         <v>1</v>
@@ -6640,10 +6654,10 @@
     </row>
     <row r="38" spans="1:8" ht="49.5">
       <c r="A38" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C38" s="10">
         <v>1</v>
@@ -6655,10 +6669,10 @@
     </row>
     <row r="39" spans="1:8" ht="33">
       <c r="A39" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" s="10">
         <v>1</v>
@@ -6670,10 +6684,10 @@
     </row>
     <row r="40" spans="1:8" ht="82.5">
       <c r="A40" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
@@ -6685,10 +6699,10 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="C41" s="10">
         <v>1</v>
@@ -6701,7 +6715,7 @@
     <row r="42" spans="1:8">
       <c r="A42" s="11"/>
       <c r="B42" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="10">
         <v>6</v>
@@ -6709,16 +6723,16 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" ht="49.5">
       <c r="A43" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" s="10">
         <v>1</v>
@@ -6728,16 +6742,16 @@
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8" ht="49.5">
       <c r="A44" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C44" s="10">
         <v>1</v>
@@ -6749,10 +6763,10 @@
     </row>
     <row r="45" spans="1:8" ht="33">
       <c r="A45" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="10">
         <v>1</v>
@@ -6765,7 +6779,7 @@
     <row r="46" spans="1:8">
       <c r="A46" s="12"/>
       <c r="B46" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="12">
         <v>2</v>
@@ -6777,10 +6791,10 @@
     </row>
     <row r="47" spans="1:8" ht="82.5">
       <c r="A47" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" s="12">
         <v>1</v>
@@ -6792,10 +6806,10 @@
     </row>
     <row r="48" spans="1:8" ht="33">
       <c r="A48" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="12">
         <v>1</v>
@@ -6807,10 +6821,10 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -6822,10 +6836,10 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
@@ -6839,10 +6853,10 @@
     </row>
     <row r="51" spans="1:8" ht="49.5">
       <c r="A51" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
@@ -6856,10 +6870,10 @@
     </row>
     <row r="52" spans="1:8" ht="33">
       <c r="A52" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
@@ -6873,10 +6887,10 @@
     </row>
     <row r="53" spans="1:8" ht="82.5">
       <c r="A53" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
@@ -6890,10 +6904,10 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
@@ -6908,7 +6922,7 @@
     <row r="55" spans="1:8">
       <c r="A55" s="12"/>
       <c r="B55" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" s="12">
         <v>6</v>
@@ -6916,16 +6930,16 @@
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" ht="49.5">
       <c r="A56" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C56" s="12">
         <v>1</v>
@@ -6935,16 +6949,16 @@
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" ht="49.5">
       <c r="A57" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -6956,10 +6970,10 @@
     </row>
     <row r="58" spans="1:8" ht="49.5">
       <c r="A58" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="12">
         <v>1</v>
@@ -6971,10 +6985,10 @@
     </row>
     <row r="59" spans="1:8" ht="33">
       <c r="A59" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -6987,7 +7001,7 @@
     <row r="60" spans="1:8">
       <c r="A60" s="9"/>
       <c r="B60" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="9">
         <v>3</v>
@@ -7067,7 +7081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17942C2D-E350-4175-91DA-E8D32862B86D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -7082,7 +7096,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7146,277 +7160,277 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="17">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="A5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
-        <v>79</v>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33">
-      <c r="A6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="33">
+      <c r="A7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="33">
+      <c r="A8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="33">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="17">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17">
+      <c r="C9" s="14">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="33">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="14">
+        <v>6</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="49.5">
+      <c r="A13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
         <v>3</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" ht="33">
-      <c r="A7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="17">
-        <v>1</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" ht="33">
-      <c r="A8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="17">
-        <v>1</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="33">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="17">
-        <v>6</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="17">
-        <v>1</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14">
         <v>2</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" ht="33">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="17">
-        <v>6</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="49.5">
-      <c r="A13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="19" t="s">
+      <c r="B17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="49.5">
+      <c r="A19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="33">
+      <c r="A20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="17">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17">
-        <v>3</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="17">
-        <v>1</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
         <v>2</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="17">
-        <v>1</v>
-      </c>
-      <c r="D15" s="17">
-        <v>3</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="17">
-        <v>1</v>
-      </c>
-      <c r="D16" s="17">
-        <v>2</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="17">
-        <v>3</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="17">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" ht="49.5">
-      <c r="A19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="17">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17">
-        <v>3</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" ht="33">
-      <c r="A20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="17">
-        <v>1</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="17">
-        <v>1</v>
-      </c>
-      <c r="D21" s="17">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14">
         <v>11</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17" t="s">
-        <v>78</v>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -7430,15 +7444,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7503,10 +7517,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7518,15 +7532,15 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7535,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7584,10 +7598,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -7598,10 +7612,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7615,7 +7629,7 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -7627,10 +7641,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -7644,7 +7658,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P1" s="1"/>
     </row>
@@ -7710,10 +7724,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7722,12 +7736,12 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -7735,10 +7749,10 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7747,30 +7761,22 @@
     <row r="8" spans="1:16">
       <c r="B8" s="2"/>
       <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="2"/>
+      <c r="C9">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>148</v>
+      <c r="F9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -7778,13 +7784,13 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
@@ -7792,13 +7798,13 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
@@ -7806,13 +7812,13 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
@@ -7820,13 +7826,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C14" s="2">
         <v>6</v>
@@ -7834,13 +7840,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2">
         <v>6</v>
@@ -7848,13 +7854,13 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -7862,13 +7868,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2">
         <v>6</v>
@@ -7876,110 +7882,117 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
+      <c r="A18" s="2"/>
+      <c r="B18" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
       <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
         <v>11</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="C23" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23">
+    <row r="24" spans="1:6">
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
     <row r="25" spans="1:6">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" s="2"/>
       <c r="C26">
-        <v>11</v>
-      </c>
-      <c r="F26" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="2"/>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" s="2"/>
@@ -8056,8 +8069,8 @@
     <row r="52" spans="2:2">
       <c r="B52" s="2"/>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="2"/>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="2"/>
@@ -8065,14 +8078,17 @@
     <row r="57" spans="2:2">
       <c r="B57" s="2"/>
     </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="2"/>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2"/>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update Save, Load (Temp)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BE8F7-563F-4F3C-9723-CB9B00F469E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF741B9F-D80B-41FE-A146-072E5AF77323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -4883,7 +4883,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4942,6 +4942,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5429,7 +5432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -7444,7 +7447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -7643,8 +7646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -7761,22 +7764,30 @@
     <row r="8" spans="1:16">
       <c r="B8" s="2"/>
       <c r="C8">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="B9" s="2"/>
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
+      <c r="A9" s="2"/>
+      <c r="B9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -7784,13 +7795,13 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
@@ -7798,13 +7809,13 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
@@ -7812,13 +7823,13 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
@@ -7826,13 +7837,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2">
         <v>6</v>
@@ -7840,13 +7851,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2">
         <v>6</v>
@@ -7854,13 +7865,13 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -7868,13 +7879,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2">
         <v>6</v>
@@ -7882,75 +7893,68 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4" t="s">
-        <v>121</v>
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
       </c>
       <c r="C18" s="2">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="2">
-        <v>4</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="C21" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="B22" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="B22" s="20"/>
       <c r="C22" s="2">
-        <v>6</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">

</xml_diff>

<commit_message>
Update Save, Load (Temp) (#76)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BE8F7-563F-4F3C-9723-CB9B00F469E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF741B9F-D80B-41FE-A146-072E5AF77323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -4883,7 +4883,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4942,6 +4942,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5429,7 +5432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEB96CA-47F2-409F-93DC-A1BA557493B6}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -7444,7 +7447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1A1C8-7761-4617-AE8A-857917D828E6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -7643,8 +7646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496AB02-A604-473C-B397-71873DC77EA1}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -7761,22 +7764,30 @@
     <row r="8" spans="1:16">
       <c r="B8" s="2"/>
       <c r="C8">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="B9" s="2"/>
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
+      <c r="A9" s="2"/>
+      <c r="B9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -7784,13 +7795,13 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
@@ -7798,13 +7809,13 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
@@ -7812,13 +7823,13 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
@@ -7826,13 +7837,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2">
         <v>6</v>
@@ -7840,13 +7851,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2">
         <v>6</v>
@@ -7854,13 +7865,13 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -7868,13 +7879,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2">
         <v>6</v>
@@ -7882,75 +7893,68 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4" t="s">
-        <v>121</v>
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
       </c>
       <c r="C18" s="2">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="2">
-        <v>4</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="C21" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="B22" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="B22" s="20"/>
       <c r="C22" s="2">
-        <v>6</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">

</xml_diff>

<commit_message>
Fix Dialogue Error (Choice, Character)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Prologue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571943F1-61AF-6449-BE30-5698B9ABDA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EE477-C415-49BB-8AE6-88FE7D4B0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -1901,7 +1901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="159">
   <si>
     <t>파일명</t>
   </si>
@@ -2393,9 +2393,6 @@
 늘 상 그랬듯이 네 선택은 곧 네 일부가 될 테니까.</t>
   </si>
   <si>
-    <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
-  </si>
-  <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 가정집 배경 속 강아지와 그 앞의 밥그릇이 보인다.</t>
   </si>
   <si>
@@ -2733,6 +2730,14 @@
   </si>
   <si>
     <t>NaruDoll:Add</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -3165,11 +3170,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
@@ -4323,16 +4328,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="77.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="48.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="48.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -5952,19 +5957,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="76.5" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -6054,9 +6061,7 @@
       <c r="C6" s="9">
         <v>11</v>
       </c>
-      <c r="D6" s="9">
-        <v>2</v>
-      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="H6" s="7"/>
@@ -6071,9 +6076,7 @@
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="9">
-        <v>3</v>
-      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="H7" s="7"/>
@@ -6201,25 +6204,23 @@
       <c r="F16" s="9"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="51.75" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" s="6">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="C18" s="6">
         <v>6</v>
@@ -6227,34 +6228,34 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="6">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C20" s="9">
         <v>1</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="9">
-        <v>2</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -6264,7 +6265,7 @@
     <row r="21" spans="1:8" ht="16.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -6277,10 +6278,10 @@
     <row r="22" spans="1:8" ht="16.5" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -6288,18 +6289,14 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="A23" s="9"/>
       <c r="B23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9">
         <v>3</v>
       </c>
+      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="H23" s="7"/>
@@ -6309,7 +6306,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -6324,7 +6321,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -6339,7 +6336,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -6354,7 +6351,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -6365,41 +6362,41 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="6">
+        <v>6</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="6">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" ht="16.5" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -6411,10 +6408,10 @@
     </row>
     <row r="31" spans="1:8" ht="16.5" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -6426,10 +6423,10 @@
     </row>
     <row r="32" spans="1:8" ht="16.5" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -6440,29 +6437,29 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="10">
-        <v>2</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -6471,10 +6468,10 @@
     </row>
     <row r="35" spans="1:8" ht="16.5" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -6486,10 +6483,10 @@
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="10">
         <v>1</v>
@@ -6501,10 +6498,10 @@
     </row>
     <row r="37" spans="1:8" ht="16.5" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C37" s="10">
         <v>1</v>
@@ -6516,10 +6513,10 @@
     </row>
     <row r="38" spans="1:8" ht="16.5" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C38" s="10">
         <v>1</v>
@@ -6531,10 +6528,10 @@
     </row>
     <row r="39" spans="1:8" ht="16.5" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="10">
         <v>1</v>
@@ -6546,10 +6543,10 @@
     </row>
     <row r="40" spans="1:8" ht="16.5" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
@@ -6561,10 +6558,10 @@
     </row>
     <row r="41" spans="1:8" ht="16.5" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C41" s="10">
         <v>1</v>
@@ -6575,36 +6572,32 @@
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A42" s="11"/>
+      <c r="A42" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="B42" s="11" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C42" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="F42" s="10"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A43" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="A43" s="11"/>
       <c r="B43" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="10">
-        <v>1</v>
-      </c>
-      <c r="D43" s="10">
-        <v>3</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="H43" s="7"/>
     </row>
@@ -6613,22 +6606,26 @@
         <v>23</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" s="10">
         <v>1</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="10">
+        <v>3</v>
+      </c>
       <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="F44" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" ht="16.5" customHeight="1">
       <c r="A45" s="10" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" s="10">
         <v>1</v>
@@ -6639,27 +6636,27 @@
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="12">
+      <c r="A46" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A47" s="12"/>
+      <c r="B47" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="12">
         <v>2</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A47" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="12">
-        <v>1</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -6668,10 +6665,10 @@
     </row>
     <row r="48" spans="1:8" ht="16.5" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C48" s="12">
         <v>1</v>
@@ -6683,10 +6680,10 @@
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1">
       <c r="A49" s="12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -6698,33 +6695,31 @@
     </row>
     <row r="50" spans="1:8" ht="16.5" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
       </c>
-      <c r="D50" s="12">
-        <v>2</v>
-      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" customHeight="1">
       <c r="A51" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
       </c>
       <c r="D51" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -6732,16 +6727,16 @@
     </row>
     <row r="52" spans="1:8" ht="16.5" customHeight="1">
       <c r="A52" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
       </c>
       <c r="D52" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -6749,16 +6744,16 @@
     </row>
     <row r="53" spans="1:8" ht="16.5" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
       </c>
       <c r="D53" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -6766,52 +6761,50 @@
     </row>
     <row r="54" spans="1:8" ht="16.5" customHeight="1">
       <c r="A54" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
       </c>
       <c r="D54" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A55" s="12"/>
+      <c r="A55" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="B55" s="13" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C55" s="12">
+        <v>1</v>
+      </c>
+      <c r="D55" s="12">
+        <v>2</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A56" s="12"/>
+      <c r="B56" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="12">
         <v>6</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A56" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="12">
-        <v>1</v>
-      </c>
-      <c r="D56" s="12">
-        <v>3</v>
-      </c>
+      <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="H56" s="7"/>
     </row>
@@ -6820,14 +6813,18 @@
         <v>23</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
       </c>
-      <c r="D57" s="12"/>
+      <c r="D57" s="12">
+        <v>3</v>
+      </c>
       <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+      <c r="F57" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" customHeight="1">
@@ -6835,7 +6832,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C58" s="12">
         <v>1</v>
@@ -6847,10 +6844,10 @@
     </row>
     <row r="59" spans="1:8" ht="16.5" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -6861,20 +6858,31 @@
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A60" s="9"/>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C61" s="9">
         <v>3</v>
       </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" ht="16.5" customHeight="1">
-      <c r="B61" s="14"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
       <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:8" ht="16.5" customHeight="1">
@@ -6907,6 +6915,7 @@
     </row>
     <row r="69" spans="2:8" ht="16.5" customHeight="1">
       <c r="B69" s="14"/>
+      <c r="H69" s="7"/>
     </row>
     <row r="70" spans="2:8" ht="16.5" customHeight="1">
       <c r="B70" s="14"/>
@@ -6932,7 +6941,9 @@
     <row r="77" spans="2:8" ht="16.5" customHeight="1">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="2:8" ht="16.5" customHeight="1"/>
+    <row r="78" spans="2:8" ht="16.5" customHeight="1">
+      <c r="B78" s="14"/>
+    </row>
     <row r="79" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="80" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="81" ht="16.5" customHeight="1"/>
@@ -7855,6 +7866,7 @@
     <row r="998" ht="16.5" customHeight="1"/>
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
+    <row r="1001" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7867,23 +7879,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -7961,7 +7973,7 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
@@ -7969,7 +7981,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="15">
         <v>1</v>
@@ -7985,7 +7997,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="15">
         <v>1</v>
@@ -7999,7 +8011,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="15">
         <v>1</v>
@@ -8011,7 +8023,7 @@
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="15">
         <v>6</v>
@@ -8019,7 +8031,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -8027,7 +8039,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
@@ -8035,7 +8047,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -8043,7 +8055,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="15">
         <v>1</v>
@@ -8065,7 +8077,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -8073,7 +8085,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
@@ -8089,7 +8101,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="15">
         <v>1</v>
@@ -8102,10 +8114,10 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
@@ -8134,7 +8146,7 @@
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
@@ -8166,10 +8178,10 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
@@ -8182,10 +8194,10 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="15">
         <v>1</v>
@@ -9214,14 +9226,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -9286,7 +9298,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
@@ -9301,7 +9313,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
@@ -9318,7 +9330,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
@@ -9367,10 +9379,10 @@
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -9384,7 +9396,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -10399,19 +10411,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="43.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P1" s="2"/>
     </row>
@@ -10477,10 +10489,10 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -10489,12 +10501,12 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1">
       <c r="B6" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -10502,10 +10514,10 @@
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -10523,7 +10535,7 @@
     <row r="9" spans="1:16" ht="16.5" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="14">
         <v>6</v>
@@ -10531,7 +10543,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1">
@@ -10545,7 +10557,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1">
@@ -10559,7 +10571,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="16.5" customHeight="1">
@@ -10573,7 +10585,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1">
@@ -10587,7 +10599,7 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1">
@@ -10601,7 +10613,7 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1">
@@ -10615,7 +10627,7 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" customHeight="1">
@@ -10629,7 +10641,7 @@
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
@@ -10643,7 +10655,7 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
@@ -10657,7 +10669,7 @@
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
@@ -10671,7 +10683,7 @@
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
@@ -10685,7 +10697,7 @@
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" customHeight="1">
@@ -10699,7 +10711,7 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
@@ -10713,7 +10725,7 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16.5" customHeight="1">
@@ -10727,7 +10739,7 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
@@ -10741,7 +10753,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" customHeight="1">
@@ -10755,7 +10767,7 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" customHeight="1">
@@ -10769,15 +10781,15 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="14">
         <v>1</v>
@@ -10795,7 +10807,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28" s="14">
         <v>1</v>
@@ -10816,13 +10828,13 @@
     </row>
     <row r="30" spans="1:6" ht="16.5" customHeight="1">
       <c r="B30" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="14">
         <v>6</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" customHeight="1">
@@ -10834,7 +10846,7 @@
     </row>
     <row r="32" spans="1:6" ht="16.5" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" s="14">
         <v>4</v>
@@ -10842,7 +10854,7 @@
     </row>
     <row r="33" spans="1:6" ht="16.5" customHeight="1">
       <c r="B33" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -10850,10 +10862,10 @@
     </row>
     <row r="34" spans="1:6" ht="16.5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Fix Dialogue Error (Choice, Character) (#94)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Prologue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571943F1-61AF-6449-BE30-5698B9ABDA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EE477-C415-49BB-8AE6-88FE7D4B0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -1901,7 +1901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="159">
   <si>
     <t>파일명</t>
   </si>
@@ -2393,9 +2393,6 @@
 늘 상 그랬듯이 네 선택은 곧 네 일부가 될 테니까.</t>
   </si>
   <si>
-    <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
-  </si>
-  <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 가정집 배경 속 강아지와 그 앞의 밥그릇이 보인다.</t>
   </si>
   <si>
@@ -2733,6 +2730,14 @@
   </si>
   <si>
     <t>NaruDoll:Add</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -3165,11 +3170,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
@@ -4323,16 +4328,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="77.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="48.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="48.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -5952,19 +5957,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="76.5" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -6054,9 +6061,7 @@
       <c r="C6" s="9">
         <v>11</v>
       </c>
-      <c r="D6" s="9">
-        <v>2</v>
-      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="H6" s="7"/>
@@ -6071,9 +6076,7 @@
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="9">
-        <v>3</v>
-      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="H7" s="7"/>
@@ -6201,25 +6204,23 @@
       <c r="F16" s="9"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="51.75" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" s="6">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="C18" s="6">
         <v>6</v>
@@ -6227,34 +6228,34 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="6">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C20" s="9">
         <v>1</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="9">
-        <v>2</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -6264,7 +6265,7 @@
     <row r="21" spans="1:8" ht="16.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -6277,10 +6278,10 @@
     <row r="22" spans="1:8" ht="16.5" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -6288,18 +6289,14 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="A23" s="9"/>
       <c r="B23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9">
         <v>3</v>
       </c>
+      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="H23" s="7"/>
@@ -6309,7 +6306,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -6324,7 +6321,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -6339,7 +6336,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -6354,7 +6351,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -6365,41 +6362,41 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="6">
+        <v>6</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="6">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" ht="16.5" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -6411,10 +6408,10 @@
     </row>
     <row r="31" spans="1:8" ht="16.5" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -6426,10 +6423,10 @@
     </row>
     <row r="32" spans="1:8" ht="16.5" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -6440,29 +6437,29 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="10">
-        <v>2</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -6471,10 +6468,10 @@
     </row>
     <row r="35" spans="1:8" ht="16.5" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -6486,10 +6483,10 @@
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="10">
         <v>1</v>
@@ -6501,10 +6498,10 @@
     </row>
     <row r="37" spans="1:8" ht="16.5" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C37" s="10">
         <v>1</v>
@@ -6516,10 +6513,10 @@
     </row>
     <row r="38" spans="1:8" ht="16.5" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C38" s="10">
         <v>1</v>
@@ -6531,10 +6528,10 @@
     </row>
     <row r="39" spans="1:8" ht="16.5" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="10">
         <v>1</v>
@@ -6546,10 +6543,10 @@
     </row>
     <row r="40" spans="1:8" ht="16.5" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
@@ -6561,10 +6558,10 @@
     </row>
     <row r="41" spans="1:8" ht="16.5" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C41" s="10">
         <v>1</v>
@@ -6575,36 +6572,32 @@
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A42" s="11"/>
+      <c r="A42" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="B42" s="11" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C42" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="F42" s="10"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A43" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="A43" s="11"/>
       <c r="B43" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="10">
-        <v>1</v>
-      </c>
-      <c r="D43" s="10">
-        <v>3</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="H43" s="7"/>
     </row>
@@ -6613,22 +6606,26 @@
         <v>23</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" s="10">
         <v>1</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="10">
+        <v>3</v>
+      </c>
       <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="F44" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" ht="16.5" customHeight="1">
       <c r="A45" s="10" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" s="10">
         <v>1</v>
@@ -6639,27 +6636,27 @@
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="12">
+      <c r="A46" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A47" s="12"/>
+      <c r="B47" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="12">
         <v>2</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A47" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="12">
-        <v>1</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -6668,10 +6665,10 @@
     </row>
     <row r="48" spans="1:8" ht="16.5" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C48" s="12">
         <v>1</v>
@@ -6683,10 +6680,10 @@
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1">
       <c r="A49" s="12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -6698,33 +6695,31 @@
     </row>
     <row r="50" spans="1:8" ht="16.5" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
       </c>
-      <c r="D50" s="12">
-        <v>2</v>
-      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" customHeight="1">
       <c r="A51" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
       </c>
       <c r="D51" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -6732,16 +6727,16 @@
     </row>
     <row r="52" spans="1:8" ht="16.5" customHeight="1">
       <c r="A52" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
       </c>
       <c r="D52" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -6749,16 +6744,16 @@
     </row>
     <row r="53" spans="1:8" ht="16.5" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
       </c>
       <c r="D53" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -6766,52 +6761,50 @@
     </row>
     <row r="54" spans="1:8" ht="16.5" customHeight="1">
       <c r="A54" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
       </c>
       <c r="D54" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A55" s="12"/>
+      <c r="A55" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="B55" s="13" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C55" s="12">
+        <v>1</v>
+      </c>
+      <c r="D55" s="12">
+        <v>2</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A56" s="12"/>
+      <c r="B56" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="12">
         <v>6</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A56" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="12">
-        <v>1</v>
-      </c>
-      <c r="D56" s="12">
-        <v>3</v>
-      </c>
+      <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="H56" s="7"/>
     </row>
@@ -6820,14 +6813,18 @@
         <v>23</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
       </c>
-      <c r="D57" s="12"/>
+      <c r="D57" s="12">
+        <v>3</v>
+      </c>
       <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+      <c r="F57" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" customHeight="1">
@@ -6835,7 +6832,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C58" s="12">
         <v>1</v>
@@ -6847,10 +6844,10 @@
     </row>
     <row r="59" spans="1:8" ht="16.5" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -6861,20 +6858,31 @@
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A60" s="9"/>
-      <c r="B60" s="8" t="s">
+      <c r="A60" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C61" s="9">
         <v>3</v>
       </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" ht="16.5" customHeight="1">
-      <c r="B61" s="14"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
       <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:8" ht="16.5" customHeight="1">
@@ -6907,6 +6915,7 @@
     </row>
     <row r="69" spans="2:8" ht="16.5" customHeight="1">
       <c r="B69" s="14"/>
+      <c r="H69" s="7"/>
     </row>
     <row r="70" spans="2:8" ht="16.5" customHeight="1">
       <c r="B70" s="14"/>
@@ -6932,7 +6941,9 @@
     <row r="77" spans="2:8" ht="16.5" customHeight="1">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="2:8" ht="16.5" customHeight="1"/>
+    <row r="78" spans="2:8" ht="16.5" customHeight="1">
+      <c r="B78" s="14"/>
+    </row>
     <row r="79" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="80" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="81" ht="16.5" customHeight="1"/>
@@ -7855,6 +7866,7 @@
     <row r="998" ht="16.5" customHeight="1"/>
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
+    <row r="1001" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7867,23 +7879,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -7961,7 +7973,7 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
@@ -7969,7 +7981,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="15">
         <v>1</v>
@@ -7985,7 +7997,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="15">
         <v>1</v>
@@ -7999,7 +8011,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="15">
         <v>1</v>
@@ -8011,7 +8023,7 @@
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="15">
         <v>6</v>
@@ -8019,7 +8031,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -8027,7 +8039,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
@@ -8035,7 +8047,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -8043,7 +8055,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="15">
         <v>1</v>
@@ -8065,7 +8077,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -8073,7 +8085,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
@@ -8089,7 +8101,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="15">
         <v>1</v>
@@ -8102,10 +8114,10 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
@@ -8134,7 +8146,7 @@
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
@@ -8166,10 +8178,10 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
@@ -8182,10 +8194,10 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="15">
         <v>1</v>
@@ -9214,14 +9226,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -9286,7 +9298,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
@@ -9301,7 +9313,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
@@ -9318,7 +9330,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
@@ -9367,10 +9379,10 @@
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -9384,7 +9396,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -10399,19 +10411,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="43.5" customWidth="1"/>
-    <col min="7" max="26" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P1" s="2"/>
     </row>
@@ -10477,10 +10489,10 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -10489,12 +10501,12 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1">
       <c r="B6" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -10502,10 +10514,10 @@
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -10523,7 +10535,7 @@
     <row r="9" spans="1:16" ht="16.5" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="14">
         <v>6</v>
@@ -10531,7 +10543,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1">
@@ -10545,7 +10557,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1">
@@ -10559,7 +10571,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="16.5" customHeight="1">
@@ -10573,7 +10585,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1">
@@ -10587,7 +10599,7 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1">
@@ -10601,7 +10613,7 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1">
@@ -10615,7 +10627,7 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" customHeight="1">
@@ -10629,7 +10641,7 @@
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
@@ -10643,7 +10655,7 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
@@ -10657,7 +10669,7 @@
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
@@ -10671,7 +10683,7 @@
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
@@ -10685,7 +10697,7 @@
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" customHeight="1">
@@ -10699,7 +10711,7 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
@@ -10713,7 +10725,7 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16.5" customHeight="1">
@@ -10727,7 +10739,7 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
@@ -10741,7 +10753,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" customHeight="1">
@@ -10755,7 +10767,7 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" customHeight="1">
@@ -10769,15 +10781,15 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="14">
         <v>1</v>
@@ -10795,7 +10807,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28" s="14">
         <v>1</v>
@@ -10816,13 +10828,13 @@
     </row>
     <row r="30" spans="1:6" ht="16.5" customHeight="1">
       <c r="B30" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="14">
         <v>6</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" customHeight="1">
@@ -10834,7 +10846,7 @@
     </row>
     <row r="32" spans="1:6" ht="16.5" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" s="14">
         <v>4</v>
@@ -10842,7 +10854,7 @@
     </row>
     <row r="33" spans="1:6" ht="16.5" customHeight="1">
       <c r="B33" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -10850,10 +10862,10 @@
     </row>
     <row r="34" spans="1:6" ht="16.5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Update Save System (Save by Room, Npc State Manage by Npc.cs)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EE477-C415-49BB-8AE6-88FE7D4B0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF89762E-2D4F-4FA7-B068-A331DBFCDEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -70,6 +71,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -95,6 +97,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -115,6 +118,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -164,6 +168,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -192,6 +197,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -217,6 +223,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -237,6 +244,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -286,6 +294,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -314,6 +323,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -339,6 +349,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -359,6 +370,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -408,6 +420,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -436,6 +449,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -461,6 +475,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1669,6 +1684,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1697,6 +1713,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1722,6 +1739,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1742,6 +1760,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1791,6 +1810,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1819,6 +1839,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1844,6 +1865,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1864,6 +1886,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1901,7 +1924,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="158">
   <si>
     <t>파일명</t>
   </si>
@@ -2705,9 +2728,6 @@
     <t>Hold, 1.5, name=Main/Stage1/#1-17</t>
   </si>
   <si>
-    <t>Hold, 1.5, name=Main/Stage1/#1-18</t>
-  </si>
-  <si>
     <t>···사, ···지··· 말라고···!!</t>
   </si>
   <si>
@@ -2715,9 +2735,6 @@
   </si>
   <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 카메라(화면)이 암전 된다.</t>
-  </si>
-  <si>
-    <t>Hold, -1, name=Main/Stage1/#1-10</t>
   </si>
   <si>
     <t>SmallRoomScene</t>
@@ -2738,6 +2755,10 @@
   </si>
   <si>
     <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, -1, name=Main/Stage1/#1-18</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -5959,7 +5980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
@@ -6213,7 +6234,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H17" s="7"/>
     </row>
@@ -6366,7 +6387,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C28" s="9">
         <v>1</v>
@@ -8047,7 +8068,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -10407,9 +10428,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P1009"/>
+  <dimension ref="A1:P1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10771,22 +10794,22 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17">
-        <v>18</v>
+      <c r="A26" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C26" s="14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14" t="s">
-        <v>148</v>
-      </c>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>149</v>
@@ -10794,132 +10817,112 @@
       <c r="C27" s="14">
         <v>1</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B28" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="14">
+        <v>6</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="14">
+        <v>5</v>
+      </c>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="14">
         <v>4</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="14">
+    </row>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B31" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14">
+    </row>
+    <row r="33" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B33" s="14"/>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B34" s="14"/>
+      <c r="C34" s="1">
         <v>11</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F34" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B30" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C30" s="14">
-        <v>6</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14">
-        <v>5</v>
-      </c>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B33" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="16.5" customHeight="1">
+    <row r="35" spans="2:6" ht="16.5" customHeight="1">
       <c r="B35" s="14"/>
-      <c r="C35" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="16.5" customHeight="1">
+    </row>
+    <row r="36" spans="2:6" ht="16.5" customHeight="1">
       <c r="B36" s="14"/>
-      <c r="C36" s="1">
-        <v>11</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="16.5" customHeight="1">
+    </row>
+    <row r="37" spans="2:6" ht="16.5" customHeight="1">
       <c r="B37" s="14"/>
     </row>
-    <row r="38" spans="1:6" ht="16.5" customHeight="1">
+    <row r="38" spans="2:6" ht="16.5" customHeight="1">
       <c r="B38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="16.5" customHeight="1">
+    <row r="39" spans="2:6" ht="16.5" customHeight="1">
       <c r="B39" s="14"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1">
+    <row r="40" spans="2:6" ht="16.5" customHeight="1">
       <c r="B40" s="14"/>
     </row>
-    <row r="41" spans="1:6" ht="16.5" customHeight="1">
+    <row r="41" spans="2:6" ht="16.5" customHeight="1">
       <c r="B41" s="14"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1">
+    <row r="42" spans="2:6" ht="16.5" customHeight="1">
       <c r="B42" s="14"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1">
+    <row r="43" spans="2:6" ht="16.5" customHeight="1">
       <c r="B43" s="14"/>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1">
+    <row r="44" spans="2:6" ht="16.5" customHeight="1">
       <c r="B44" s="14"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1">
+    <row r="45" spans="2:6" ht="16.5" customHeight="1">
       <c r="B45" s="14"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1">
+    <row r="46" spans="2:6" ht="16.5" customHeight="1">
       <c r="B46" s="14"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1">
+    <row r="47" spans="2:6" ht="16.5" customHeight="1">
       <c r="B47" s="14"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1">
+    <row r="48" spans="2:6" ht="16.5" customHeight="1">
       <c r="B48" s="14"/>
     </row>
     <row r="49" spans="2:2" ht="16.5" customHeight="1">
@@ -10958,34 +10961,30 @@
     <row r="60" spans="2:2" ht="16.5" customHeight="1">
       <c r="B60" s="14"/>
     </row>
-    <row r="61" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B61" s="14"/>
-    </row>
-    <row r="62" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B62" s="14"/>
-    </row>
-    <row r="63" spans="2:2" ht="16.5" customHeight="1"/>
-    <row r="64" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="61" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="62" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="63" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B63" s="14"/>
+    </row>
+    <row r="64" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B64" s="14"/>
+    </row>
     <row r="65" spans="2:2" ht="16.5" customHeight="1">
       <c r="B65" s="14"/>
     </row>
-    <row r="66" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B66" s="14"/>
-    </row>
-    <row r="67" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B67" s="14"/>
-    </row>
-    <row r="68" spans="2:2" ht="16.5" customHeight="1"/>
-    <row r="69" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="66" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="67" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="68" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B68" s="14"/>
+    </row>
+    <row r="69" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B69" s="14"/>
+    </row>
     <row r="70" spans="2:2" ht="16.5" customHeight="1">
       <c r="B70" s="14"/>
     </row>
-    <row r="71" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B71" s="14"/>
-    </row>
-    <row r="72" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B72" s="14"/>
-    </row>
+    <row r="71" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="72" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="73" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="74" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="75" spans="2:2" ht="16.5" customHeight="1"/>
@@ -11921,8 +11920,6 @@
     <row r="1005" ht="16.5" customHeight="1"/>
     <row r="1006" ht="16.5" customHeight="1"/>
     <row r="1007" ht="16.5" customHeight="1"/>
-    <row r="1008" ht="16.5" customHeight="1"/>
-    <row r="1009" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Update Save System (Save by Room, Npc State Manage by Npc.cs) (#112)
* Update Save System (Save by Room, Npc State Manage by Npc.cs)

* Merge branch 'dev' into Feature/CP-95
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EE477-C415-49BB-8AE6-88FE7D4B0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF89762E-2D4F-4FA7-B068-A331DBFCDEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -70,6 +71,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -95,6 +97,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -115,6 +118,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -164,6 +168,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -192,6 +197,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -217,6 +223,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -237,6 +244,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -286,6 +294,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -314,6 +323,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -339,6 +349,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -359,6 +370,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -408,6 +420,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -436,6 +449,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -461,6 +475,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1669,6 +1684,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1697,6 +1713,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1722,6 +1739,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1742,6 +1760,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1791,6 +1810,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1819,6 +1839,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1844,6 +1865,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1864,6 +1886,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -1901,7 +1924,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="158">
   <si>
     <t>파일명</t>
   </si>
@@ -2705,9 +2728,6 @@
     <t>Hold, 1.5, name=Main/Stage1/#1-17</t>
   </si>
   <si>
-    <t>Hold, 1.5, name=Main/Stage1/#1-18</t>
-  </si>
-  <si>
     <t>···사, ···지··· 말라고···!!</t>
   </si>
   <si>
@@ -2715,9 +2735,6 @@
   </si>
   <si>
     <t>(컷 씬)&gt; (컷 씬 전환): 카메라(화면)이 암전 된다.</t>
-  </si>
-  <si>
-    <t>Hold, -1, name=Main/Stage1/#1-10</t>
   </si>
   <si>
     <t>SmallRoomScene</t>
@@ -2738,6 +2755,10 @@
   </si>
   <si>
     <t>말이 길어졌네. 직접 보여 줄게. 그래. 네 앞에 강아지, 보이지?</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, -1, name=Main/Stage1/#1-18</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -5959,7 +5980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
@@ -6213,7 +6234,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H17" s="7"/>
     </row>
@@ -6366,7 +6387,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C28" s="9">
         <v>1</v>
@@ -8047,7 +8068,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -10407,9 +10428,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P1009"/>
+  <dimension ref="A1:P1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10771,22 +10794,22 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17">
-        <v>18</v>
+      <c r="A26" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C26" s="14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14" t="s">
-        <v>148</v>
-      </c>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>149</v>
@@ -10794,132 +10817,112 @@
       <c r="C27" s="14">
         <v>1</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B28" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="14">
+        <v>6</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="14">
+        <v>5</v>
+      </c>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="14">
         <v>4</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="14">
+    </row>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B31" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14">
+    </row>
+    <row r="33" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B33" s="14"/>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B34" s="14"/>
+      <c r="C34" s="1">
         <v>11</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F34" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B30" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C30" s="14">
-        <v>6</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14">
-        <v>5</v>
-      </c>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B33" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="16.5" customHeight="1">
+    <row r="35" spans="2:6" ht="16.5" customHeight="1">
       <c r="B35" s="14"/>
-      <c r="C35" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="16.5" customHeight="1">
+    </row>
+    <row r="36" spans="2:6" ht="16.5" customHeight="1">
       <c r="B36" s="14"/>
-      <c r="C36" s="1">
-        <v>11</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="16.5" customHeight="1">
+    </row>
+    <row r="37" spans="2:6" ht="16.5" customHeight="1">
       <c r="B37" s="14"/>
     </row>
-    <row r="38" spans="1:6" ht="16.5" customHeight="1">
+    <row r="38" spans="2:6" ht="16.5" customHeight="1">
       <c r="B38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="16.5" customHeight="1">
+    <row r="39" spans="2:6" ht="16.5" customHeight="1">
       <c r="B39" s="14"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1">
+    <row r="40" spans="2:6" ht="16.5" customHeight="1">
       <c r="B40" s="14"/>
     </row>
-    <row r="41" spans="1:6" ht="16.5" customHeight="1">
+    <row r="41" spans="2:6" ht="16.5" customHeight="1">
       <c r="B41" s="14"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1">
+    <row r="42" spans="2:6" ht="16.5" customHeight="1">
       <c r="B42" s="14"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1">
+    <row r="43" spans="2:6" ht="16.5" customHeight="1">
       <c r="B43" s="14"/>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1">
+    <row r="44" spans="2:6" ht="16.5" customHeight="1">
       <c r="B44" s="14"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1">
+    <row r="45" spans="2:6" ht="16.5" customHeight="1">
       <c r="B45" s="14"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1">
+    <row r="46" spans="2:6" ht="16.5" customHeight="1">
       <c r="B46" s="14"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1">
+    <row r="47" spans="2:6" ht="16.5" customHeight="1">
       <c r="B47" s="14"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1">
+    <row r="48" spans="2:6" ht="16.5" customHeight="1">
       <c r="B48" s="14"/>
     </row>
     <row r="49" spans="2:2" ht="16.5" customHeight="1">
@@ -10958,34 +10961,30 @@
     <row r="60" spans="2:2" ht="16.5" customHeight="1">
       <c r="B60" s="14"/>
     </row>
-    <row r="61" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B61" s="14"/>
-    </row>
-    <row r="62" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B62" s="14"/>
-    </row>
-    <row r="63" spans="2:2" ht="16.5" customHeight="1"/>
-    <row r="64" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="61" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="62" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="63" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B63" s="14"/>
+    </row>
+    <row r="64" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B64" s="14"/>
+    </row>
     <row r="65" spans="2:2" ht="16.5" customHeight="1">
       <c r="B65" s="14"/>
     </row>
-    <row r="66" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B66" s="14"/>
-    </row>
-    <row r="67" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B67" s="14"/>
-    </row>
-    <row r="68" spans="2:2" ht="16.5" customHeight="1"/>
-    <row r="69" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="66" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="67" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="68" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B68" s="14"/>
+    </row>
+    <row r="69" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B69" s="14"/>
+    </row>
     <row r="70" spans="2:2" ht="16.5" customHeight="1">
       <c r="B70" s="14"/>
     </row>
-    <row r="71" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B71" s="14"/>
-    </row>
-    <row r="72" spans="2:2" ht="16.5" customHeight="1">
-      <c r="B72" s="14"/>
-    </row>
+    <row r="71" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="72" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="73" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="74" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="75" spans="2:2" ht="16.5" customHeight="1"/>
@@ -11921,8 +11920,6 @@
     <row r="1005" ht="16.5" customHeight="1"/>
     <row r="1006" ht="16.5" customHeight="1"/>
     <row r="1007" ht="16.5" customHeight="1"/>
-    <row r="1008" ht="16.5" customHeight="1"/>
-    <row r="1009" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Add Stage 2 - Excel, Scene(Temp), Script (Item, Dialogue, Interaction)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Prologue/prologue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Prologue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Prologue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF89762E-2D4F-4FA7-B068-A331DBFCDEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA99E4D6-E7DC-AF43-832A-BD069CF7B18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="prologue 3" sheetId="4" r:id="rId4"/>
     <sheet name="naru iteration" sheetId="5" r:id="rId5"/>
     <sheet name="story1 interaction" sheetId="6" r:id="rId6"/>
+    <sheet name="story2 interaction" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -1923,8 +1924,723 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{DC98ACF2-BED8-C444-9558-E29C34BFE33A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAAzX7jpX4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UISU    (2023-06-15 23:16:56)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">0: NONE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>대화</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>선택지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (1, 2, 3)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>선택지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>종료</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>맵</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>이동</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>이동할</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>이름</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - contents)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5: Save
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">9: Random
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">10: Random End
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>11: Immediately Execute (</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>대사</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>없이</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>바로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>캐릭터</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> State</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>변경하는</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>용도로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>사용합니다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>. ex) Left, Appear</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>와</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Right, Appear</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>동시에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>사용하고</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>싶은</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>경우</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>// Inspector</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>창에서</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>직접</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>조정</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6: CutScene
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">7: WaitInteract
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>8: Interact</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{05BC1AC9-EF5F-B34C-B978-34EEE54880D0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzX7jpW8
+UISU    (2023-06-15 23:16:56)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{B296DB4A-EAA0-A641-88CE-10C2E7418941}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzX7jpX8
+UISU    (2023-06-15 23:16:56)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{8B8285D2-A0A7-5046-827B-03A458AF0776}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzX7jpYA
+서 의수    (2023-06-15 23:16:56)
+이미 사용하고 있는 구분자
+:, ()
+- 아이템 획득, 수거 (모든 타입에서 가능. 단, 일부 (Random 혹은 Choice 관련 안됨.))
+v0 : v1 (여러개 가능 - ex) Bag:Add, Cap:Add)
+v0 - Item name
+v1 - Add, Remove
+- 1 (Script)
+0: 스킵 불가능
+1(value) : {$value}배속
+- 캐릭터 등장 (Script, ImmediatelyExecute에서 가능)
+v0, v1 (순서 무관)
+v0 - Left, Right
+v1 - Appear, Active, Inactive, Disappear
+- 컷씬
+v0, v1, v2, v3 (순서 무관)
+v0 - Hold, None (Default - None)   (대소문자 무관)
+v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
+v2 - True, False 다음 Index로 Auto 여부 (Default - True)  (대소문자 무관)
+v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="181">
   <si>
     <t>파일명</t>
   </si>
@@ -2761,12 +3477,123 @@
     <t>Hold, -1, name=Main/Stage1/#1-18</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
+  <si>
+    <t>아이</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>아니.</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>별 일도 아닌 걸로 귀찮게 굴지 마.</t>
+  </si>
+  <si>
+    <t>이야기를 들려줘.</t>
+  </si>
+  <si>
+    <t>내 이야기를 들려 달라고?
+너도 참 별종이구나.</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage2 - 아이</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토리필드(??)</t>
+  </si>
+  <si>
+    <t>스토리필드(??)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 3, name=Main/Stage2/#1-1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-4</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-5</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-6</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-7</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-8</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-9</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-10</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-11</t>
+  </si>
+  <si>
+    <t>Hold, 1.5, name=Main/Stage2/#1-12</t>
+  </si>
+  <si>
+    <t>Hold, -1, name=Main/Stage2/#1-13</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>뭐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="A고딕12"/>
+      </rPr>
+      <t>···</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 할 말이라도 있어?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>···</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>좋아. 재미없다고 투정 부리지나 마.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2833,6 +3660,31 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="A고딕12"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2914,7 +3766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2968,6 +3820,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3191,11 +4058,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1">
@@ -4351,14 +5218,14 @@
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="48.5" customWidth="1"/>
+    <col min="7" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -5984,15 +6851,15 @@
       <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="76.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="76.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -7904,14 +8771,14 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="80.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="80.5" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -9247,9 +10114,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -10430,18 +11297,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="84.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="43.5" customWidth="1"/>
+    <col min="7" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -11926,4 +12793,387 @@
   <pageSetup orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEC236A-617C-7443-94AF-72164B656E6B}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.5" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32">
+      <c r="A7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>6</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>6</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="14"/>
+      <c r="B12" s="17">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14">
+        <v>6</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14">
+        <v>6</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17">
+        <v>5</v>
+      </c>
+      <c r="C14" s="14">
+        <v>6</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17">
+        <v>6</v>
+      </c>
+      <c r="C15" s="14">
+        <v>6</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14">
+        <v>6</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14">
+        <v>6</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18">
+      <c r="A18" s="14"/>
+      <c r="B18" s="17">
+        <v>9</v>
+      </c>
+      <c r="C18" s="14">
+        <v>6</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17">
+        <v>10</v>
+      </c>
+      <c r="C19" s="14">
+        <v>6</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18">
+      <c r="A20" s="14"/>
+      <c r="B20" s="17">
+        <v>11</v>
+      </c>
+      <c r="C20" s="14">
+        <v>6</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17">
+        <v>12</v>
+      </c>
+      <c r="C21" s="14">
+        <v>6</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17">
+        <v>13</v>
+      </c>
+      <c r="C22" s="14">
+        <v>6</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17">
+      <c r="A23" s="14"/>
+      <c r="B23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="14">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="17">
+      <c r="A24" s="14"/>
+      <c r="B24" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="14">
+        <v>4</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" ht="18">
+      <c r="B25" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17">
+      <c r="A26" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17">
+      <c r="B27" s="14"/>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17">
+      <c r="B28" s="14"/>
+      <c r="C28" s="1">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>